<commit_message>
**REQUIREMENT**: openpyxl now needed; allows spreadsheet storage of component parameters that's easy to edit - Added PackageDimensioning: Creates package dimensions from a spreadsheet - Added pthPad: Creates plated through-hole pads based on IPC2222 specifications - Started adding test stuff - Cleaned up a lot of ssop.py - Added roundrect pad shape to Pad.py - Added trapezoid delta to Pad.py - Added SMD parameter based pad creation based on IPC7351C - Added both GullWingParams and JointParams spreadsheets that cover the necessary parameters to build footprints from
</commit_message>
<xml_diff>
--- a/KicadModTree/JointParams.xlsx
+++ b/KicadModTree/JointParams.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chip" sheetId="5" r:id="rId1"/>
@@ -213,10 +213,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,24 +544,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -614,40 +614,40 @@
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="C3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>-0.05</v>
       </c>
-      <c r="F3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="1">
         <v>0.5</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.6</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
         <v>0.05</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -658,40 +658,40 @@
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.3</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>-0.05</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="F4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.5</v>
       </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
         <v>0.05</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -702,40 +702,40 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>-0.05</v>
       </c>
-      <c r="F5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.35</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.45</v>
       </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
         <v>0.05</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -746,40 +746,40 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
         <v>-0.05</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.3</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>0.05</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -790,40 +790,40 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.15</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>-0.02</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>-0.02</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="F7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="1">
         <v>-0.01</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>-0.01</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>0.15</v>
       </c>
-      <c r="K7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="K7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -834,40 +834,40 @@
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.08</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>-0.03</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>-0.03</v>
       </c>
-      <c r="F8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="F8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1">
         <v>-0.02</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>-0.02</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>0.15</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>0.12</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>-0.01</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>-0.01</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -878,40 +878,40 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.04</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>-0.04</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>-0.04</v>
       </c>
-      <c r="F9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.05</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>-0.03</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>-0.03</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>0.15</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>0.06</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>-0.02</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>-0.02</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -929,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -960,189 +960,189 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.75</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.65</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0.45</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.6</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.45</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.5</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="1">
         <v>0.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0.45</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.45</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.35</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>0.3</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="B9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.3</v>
       </c>
-      <c r="E9" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="1">
         <v>0.35</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.35</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>0.23</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>0.33</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.3</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="C11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="1">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="B12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="1">
         <v>0.17</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="1">
         <v>0.15</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.17</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -1155,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="B1:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,24 +1168,24 @@
       <c r="A1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1232,40 +1232,40 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.3</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.05</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.35</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.45</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.06</v>
       </c>
-      <c r="I3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.5</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1273,40 +1273,40 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.35</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.04</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.3</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="G4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.05</v>
       </c>
-      <c r="I4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.35</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>0.45</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>0.06</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1314,40 +1314,40 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.03</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.35</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0.04</v>
       </c>
-      <c r="I5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.3</v>
       </c>
-      <c r="K5" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="K5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L5" s="1">
         <v>0.05</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1355,40 +1355,40 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.15</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.01</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="E6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.35</v>
       </c>
-      <c r="L6" s="2">
+      <c r="G6" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.03</v>
       </c>
-      <c r="M6" s="2">
+      <c r="I6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M6" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1396,40 +1396,40 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="1">
         <v>-0.02</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.15</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="1">
         <v>-0.01</v>
       </c>
-      <c r="I7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="I7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="1">
         <v>0.3</v>
       </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1437,40 +1437,40 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="B8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1">
         <v>-0.03</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.15</v>
       </c>
-      <c r="G8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="1">
         <v>-0.02</v>
       </c>
-      <c r="I8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="I8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="1">
         <v>0.3</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>-0.01</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1501,24 +1501,24 @@
       <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1565,40 +1565,40 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.05</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="1">
         <v>0.35</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.06</v>
       </c>
-      <c r="I3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.3</v>
       </c>
-      <c r="K3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="K3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L3" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1606,40 +1606,40 @@
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.15</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.04</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1">
         <v>0.5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.05</v>
       </c>
-      <c r="I4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="I4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.3</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>0.06</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1647,40 +1647,40 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.15</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.03</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.04</v>
       </c>
-      <c r="I5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="I5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.3</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>0.05</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1688,40 +1688,40 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.15</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.01</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.15</v>
       </c>
-      <c r="G6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="G6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.02</v>
       </c>
-      <c r="I6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1">
         <v>0.02</v>
       </c>
-      <c r="K6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="K6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L6" s="1">
         <v>0.03</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1729,40 +1729,40 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.15</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>-0.02</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.15</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="1">
         <v>-0.01</v>
       </c>
-      <c r="I7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="I7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1770,40 +1770,40 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.15</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>-0.03</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.15</v>
       </c>
-      <c r="G8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="1">
         <v>-0.02</v>
       </c>
-      <c r="I8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="I8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L8" s="1">
         <v>-0.01</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1834,24 +1834,24 @@
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1898,40 +1898,40 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.35</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.15</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.45</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.5</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="H3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>0.6</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>0.3</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1939,40 +1939,40 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.35</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="C4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.45</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.15</v>
       </c>
-      <c r="I4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>0.6</v>
       </c>
-      <c r="L4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="L4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="M4" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -1980,40 +1980,40 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.05</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
         <v>0.35</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>0.5</v>
       </c>
-      <c r="H5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="H5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.45</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>0.6</v>
       </c>
-      <c r="L5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="L5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -2021,40 +2021,40 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.35</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.45</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0.05</v>
       </c>
-      <c r="I6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="I6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K6" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="L6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -2062,40 +2062,40 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.3</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.05</v>
       </c>
-      <c r="I7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1">
         <v>0.35</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>0.5</v>
       </c>
-      <c r="L7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="L7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M7" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -2129,24 +2129,24 @@
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2193,40 +2193,40 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.05</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="1">
         <v>0.35</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.06</v>
       </c>
-      <c r="I3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.3</v>
       </c>
-      <c r="K3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="K3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L3" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>